<commit_message>
Mudanças pontuais e contextos
</commit_message>
<xml_diff>
--- a/docs/Local_Equip._e_Dispositivos_TI (1).xlsx
+++ b/docs/Local_Equip._e_Dispositivos_TI (1).xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64aa966fd3204f76/Documentos/GitHub/SK_FLOW_gestaoChamatosTI-UNIKA/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB799214-B199-407D-BC97-CD62FCBBF94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{CB799214-B199-407D-BC97-CD62FCBBF94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6203B664-646A-4A1B-80B9-3F6D168DDD52}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="228" windowWidth="30936" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="new sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="IMPORTADO" sheetId="2" r:id="rId1"/>
+    <sheet name="new sheet" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="133">
   <si>
     <t>Código</t>
   </si>
@@ -392,6 +406,33 @@
   </si>
   <si>
     <t>IMPRESSORA LASER</t>
+  </si>
+  <si>
+    <t>CODPROD</t>
+  </si>
+  <si>
+    <t>CODUSU</t>
+  </si>
+  <si>
+    <t>CODLOCAL</t>
+  </si>
+  <si>
+    <t>STATUSUSO</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>DATAINI</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>NUM_SERIE</t>
+  </si>
+  <si>
+    <t>OBSTECNICA</t>
   </si>
 </sst>
 </file>
@@ -809,11 +850,1309 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66CE987-E20B-499C-9615-01FF69A2AD81}">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>20160000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>20020000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>20160000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>20060000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>20160000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>20160000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>20030000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>20030000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>20160000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>20160000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>20160000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>20160000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>20160000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>20160000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>20160000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>20140000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>20140000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>20160000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>20160000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>20160000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>20160000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>20160000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>20160000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>20160000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>20160000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>20160000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>20160000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F28" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>20100000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>20160000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>20160000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>20160000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F32" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>20160000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>20160000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F34" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>20160000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>20160000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>20160000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F37" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>20160000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>20160000</v>
+      </c>
+      <c r="D39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F39" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>20160000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F40" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>25</v>
+      </c>
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>20160000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>20160000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>20160000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F43" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>20160000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F44" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>20160000</v>
+      </c>
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>25</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>20160000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>59</v>
+      </c>
+      <c r="H46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>20160000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>20160000</v>
+      </c>
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F48" t="s">
+        <v>115</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>20160000</v>
+      </c>
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="2">
+        <v>45658</v>
+      </c>
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>